<commit_message>
Add profile update functionality
+update method
+profile template modified
+update routes
+searchFor method (no routes or views implemented)
</commit_message>
<xml_diff>
--- a/public/import/employees-list.xlsx
+++ b/public/import/employees-list.xlsx
@@ -1,37 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20339"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JARO\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{308D5ED6-CB29-4DEE-AD85-497F67DD3242}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Worksheet" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029" forceFullCalc="1"/>
+  <definedNames/>
+  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1" forceFullCalc="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="33">
   <si>
     <t>Airi Satou</t>
   </si>
   <si>
-    <t>Accountant</t>
+    <t>Account man</t>
   </si>
   <si>
     <t>Tokyo</t>
   </si>
   <si>
-    <t>2023-02-12T19:32:10.000000Z</t>
+    <t>2023-02-19T01:00:19.000000Z</t>
   </si>
   <si>
     <t>Angelica Ramos</t>
@@ -43,36 +38,24 @@
     <t>London</t>
   </si>
   <si>
-    <t>2023-02-12T19:34:03.000000Z</t>
-  </si>
-  <si>
     <t>Ashton Cox</t>
   </si>
   <si>
-    <t>Junior Technical Author</t>
+    <t>Technical Author</t>
   </si>
   <si>
     <t>San Francisco</t>
   </si>
   <si>
-    <t>2023-02-12T19:35:40.000000Z</t>
-  </si>
-  <si>
     <t>Bradley Greer</t>
   </si>
   <si>
     <t>Software Engineer</t>
   </si>
   <si>
-    <t>2023-02-12T19:40:32.000000Z</t>
-  </si>
-  <si>
     <t>Brenden Wagner</t>
   </si>
   <si>
-    <t>2023-02-12T19:41:33.000000Z</t>
-  </si>
-  <si>
     <t>Brielle Williamson</t>
   </si>
   <si>
@@ -82,66 +65,68 @@
     <t>New York</t>
   </si>
   <si>
-    <t>2023-02-12T19:42:32.000000Z</t>
-  </si>
-  <si>
     <t>Bruno Nash</t>
   </si>
   <si>
-    <t>2023-02-12T19:43:22.000000Z</t>
-  </si>
-  <si>
     <t>Newman</t>
   </si>
   <si>
     <t>Laravel Developer</t>
   </si>
   <si>
-    <t>2023-02-12T20:10:04.000000Z</t>
-  </si>
-  <si>
     <t>Altair Fred</t>
   </si>
   <si>
     <t>QA</t>
   </si>
   <si>
-    <t>2023-02-12T20:12:12.000000Z</t>
-  </si>
-  <si>
     <t>Yee Pee</t>
   </si>
   <si>
     <t>Junior Java Developer</t>
   </si>
   <si>
-    <t>2023-02-12T20:16:26.000000Z</t>
-  </si>
-  <si>
     <t>Robert Jr</t>
   </si>
   <si>
     <t>Senior Laravel Developer</t>
   </si>
   <si>
-    <t>2023-02-12T20:21:20.000000Z</t>
-  </si>
-  <si>
     <t>Joseph A</t>
   </si>
   <si>
     <t>Junior Laravel Developer</t>
   </si>
   <si>
-    <t>2023-02-12T20:23:19.000000Z</t>
+    <t>Sernosh Ulianof</t>
+  </si>
+  <si>
+    <t>Trainer</t>
+  </si>
+  <si>
+    <t>Chicago</t>
+  </si>
+  <si>
+    <t>2023-02-19T14:19:33.000000Z</t>
+  </si>
+  <si>
+    <t>Matt Jinxer</t>
+  </si>
+  <si>
+    <t>2023-02-19T14:23:18.000000Z</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -156,33 +141,21 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
 </styleSheet>
 </file>
 
@@ -472,22 +445,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="20.140625" customWidth="1"/>
-    <col min="3" max="3" width="25.140625" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
-    <col min="6" max="6" width="27.140625" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1">
         <v>1</v>
       </c>
@@ -507,10 +477,10 @@
         <v>3</v>
       </c>
       <c r="G1">
-        <v>1627</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1627.0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>2</v>
       </c>
@@ -527,44 +497,44 @@
         <v>47</v>
       </c>
       <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2">
+        <v>62200.0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="G2">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
       </c>
       <c r="E3">
         <v>66</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="G3">
-        <v>86000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3000.0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -573,67 +543,67 @@
         <v>41</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="G4">
-        <v>13200</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>13200.0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E5">
         <v>28</v>
       </c>
       <c r="F5" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="G5">
-        <v>20680</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>20680.0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E6">
         <v>61</v>
       </c>
       <c r="F6" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="G6">
-        <v>37200</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>37200.0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D7" t="s">
         <v>6</v>
@@ -642,21 +612,21 @@
         <v>38</v>
       </c>
       <c r="F7" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="G7">
-        <v>16350</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>16350.0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
         <v>6</v>
@@ -665,44 +635,44 @@
         <v>34</v>
       </c>
       <c r="F8" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="G8">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1000.0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E9">
         <v>40</v>
       </c>
       <c r="F9" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="G9">
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2500.0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D10" t="s">
         <v>2</v>
@@ -711,59 +681,116 @@
         <v>20</v>
       </c>
       <c r="F10" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="G10">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1500.0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E11">
         <v>39</v>
       </c>
       <c r="F11" t="s">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="G11">
-        <v>19000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>19000.0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="D12" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E12">
         <v>34</v>
       </c>
       <c r="F12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12">
+        <v>4000.0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13">
+        <v>45</v>
+      </c>
+      <c r="F13" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13">
+        <v>4000.0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14">
         <v>37</v>
       </c>
-      <c r="G12">
-        <v>2000</v>
+      <c r="F14" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14">
+        <v>5500.0</v>
       </c>
     </row>
   </sheetData>
+  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+  <tableParts count="0"/>
 </worksheet>
 </file>
</xml_diff>